<commit_message>
Added XML data generator to generate from xml file
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/xmlTestData1.xlsx
+++ b/src/test/resources/configs/data/xmlTestData1.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="157">
   <si>
     <t>Key</t>
   </si>
@@ -488,6 +488,12 @@
   </si>
   <si>
     <t>123 Production Address++ Shenzhen++ China.</t>
+  </si>
+  <si>
+    <t>invalid.product.1</t>
+  </si>
+  <si>
+    <t>IMPORTER</t>
   </si>
 </sst>
 </file>
@@ -1351,7 +1357,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1385,7 +1391,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>156</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -1461,7 +1467,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1514,7 +1520,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F2">
         <v>10</v>
@@ -1533,7 +1539,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1551,7 +1557,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2125,7 +2131,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>